<commit_message>
added ReadMe.md & updated components/function.js
</commit_message>
<xml_diff>
--- a/2024.xlsx
+++ b/2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Development\NodeJS ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F6FED2-7D58-4ADA-84A7-2E73E003B4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{855C1EA6-AB47-4E16-AC86-F157CE42453D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="5892" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Income" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4207" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4207" uniqueCount="154">
   <si>
     <t>income list for the period January 1, 2024 – January 1, 2025</t>
   </si>
@@ -485,9 +485,6 @@
   <si>
     <t>Incoming currency</t>
   </si>
-  <si>
-    <t>sda</t>
-  </si>
 </sst>
 </file>
 
@@ -749,9 +746,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,7 +762,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -810,12 +807,12 @@
   <dimension ref="A1:J524"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -829,7 +826,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -840,7 +837,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -861,7 +858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -893,7 +890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -925,7 +922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -957,7 +954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -989,7 +986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1021,7 +1018,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1053,7 +1050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1085,7 +1082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1117,7 +1114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1149,7 +1146,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1181,7 +1178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1213,7 +1210,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1245,7 +1242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1277,7 +1274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1309,7 +1306,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1341,7 +1338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1373,7 +1370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1405,7 +1402,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1437,7 +1434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1469,7 +1466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1501,7 +1498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1533,7 +1530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1565,7 +1562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1597,7 +1594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1629,7 +1626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1661,7 +1658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -1693,7 +1690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1725,7 +1722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1757,7 +1754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -1789,7 +1786,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -1821,7 +1818,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>26</v>
       </c>
@@ -1853,7 +1850,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1885,7 +1882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -1917,7 +1914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -1949,7 +1946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>27</v>
       </c>
@@ -1981,7 +1978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>27</v>
       </c>
@@ -2013,7 +2010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>27</v>
       </c>
@@ -2045,7 +2042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>27</v>
       </c>
@@ -2077,7 +2074,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>30</v>
       </c>
@@ -2109,7 +2106,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -2141,7 +2138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>30</v>
       </c>
@@ -2173,7 +2170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>30</v>
       </c>
@@ -2205,7 +2202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>30</v>
       </c>
@@ -2237,7 +2234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -2269,7 +2266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -2301,7 +2298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -2333,7 +2330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -2365,7 +2362,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -2397,7 +2394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -2429,7 +2426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -2461,7 +2458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>32</v>
       </c>
@@ -2493,7 +2490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>32</v>
       </c>
@@ -2525,7 +2522,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>32</v>
       </c>
@@ -2557,7 +2554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>32</v>
       </c>
@@ -2589,7 +2586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>32</v>
       </c>
@@ -2621,7 +2618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>32</v>
       </c>
@@ -2653,7 +2650,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>33</v>
       </c>
@@ -2685,7 +2682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>33</v>
       </c>
@@ -2717,7 +2714,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>33</v>
       </c>
@@ -2749,7 +2746,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>33</v>
       </c>
@@ -2781,7 +2778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>34</v>
       </c>
@@ -2813,7 +2810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>34</v>
       </c>
@@ -2845,7 +2842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>34</v>
       </c>
@@ -2877,7 +2874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>34</v>
       </c>
@@ -2909,7 +2906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -2941,7 +2938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -2973,7 +2970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>34</v>
       </c>
@@ -3005,7 +3002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>36</v>
       </c>
@@ -3037,7 +3034,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>36</v>
       </c>
@@ -3069,7 +3066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>36</v>
       </c>
@@ -3101,7 +3098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>36</v>
       </c>
@@ -3133,7 +3130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>36</v>
       </c>
@@ -3165,7 +3162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>36</v>
       </c>
@@ -3197,7 +3194,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>36</v>
       </c>
@@ -3229,7 +3226,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>36</v>
       </c>
@@ -3261,7 +3258,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>37</v>
       </c>
@@ -3293,7 +3290,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>37</v>
       </c>
@@ -3325,7 +3322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>37</v>
       </c>
@@ -3357,7 +3354,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>37</v>
       </c>
@@ -3389,7 +3386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>38</v>
       </c>
@@ -3421,7 +3418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>38</v>
       </c>
@@ -3453,7 +3450,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>38</v>
       </c>
@@ -3485,7 +3482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>38</v>
       </c>
@@ -3517,7 +3514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>38</v>
       </c>
@@ -3549,7 +3546,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>39</v>
       </c>
@@ -3581,7 +3578,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>39</v>
       </c>
@@ -3613,7 +3610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>39</v>
       </c>
@@ -3645,7 +3642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>39</v>
       </c>
@@ -3677,7 +3674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>39</v>
       </c>
@@ -3709,7 +3706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>40</v>
       </c>
@@ -3741,7 +3738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>40</v>
       </c>
@@ -3773,7 +3770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>40</v>
       </c>
@@ -3805,7 +3802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="95" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>40</v>
       </c>
@@ -3837,7 +3834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>40</v>
       </c>
@@ -3869,7 +3866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>40</v>
       </c>
@@ -3901,7 +3898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>40</v>
       </c>
@@ -3933,7 +3930,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="99" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>40</v>
       </c>
@@ -3965,7 +3962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>40</v>
       </c>
@@ -3997,7 +3994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>42</v>
       </c>
@@ -4029,7 +4026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>42</v>
       </c>
@@ -4061,7 +4058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>42</v>
       </c>
@@ -4093,7 +4090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="104" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>42</v>
       </c>
@@ -4125,7 +4122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="105" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>42</v>
       </c>
@@ -4157,7 +4154,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>43</v>
       </c>
@@ -4189,7 +4186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>43</v>
       </c>
@@ -4221,7 +4218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>43</v>
       </c>
@@ -4253,7 +4250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>43</v>
       </c>
@@ -4285,7 +4282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>43</v>
       </c>
@@ -4317,7 +4314,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>44</v>
       </c>
@@ -4349,7 +4346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>44</v>
       </c>
@@ -4381,7 +4378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="113" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>44</v>
       </c>
@@ -4413,7 +4410,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="114" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>44</v>
       </c>
@@ -4445,7 +4442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>45</v>
       </c>
@@ -4477,7 +4474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>45</v>
       </c>
@@ -4509,7 +4506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>45</v>
       </c>
@@ -4541,7 +4538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>45</v>
       </c>
@@ -4573,7 +4570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="119" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>45</v>
       </c>
@@ -4605,7 +4602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>46</v>
       </c>
@@ -4637,7 +4634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>46</v>
       </c>
@@ -4669,7 +4666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>46</v>
       </c>
@@ -4701,7 +4698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="123" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>46</v>
       </c>
@@ -4733,7 +4730,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="124" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>48</v>
       </c>
@@ -4765,7 +4762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>48</v>
       </c>
@@ -4797,7 +4794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>48</v>
       </c>
@@ -4829,7 +4826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="127" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>48</v>
       </c>
@@ -4861,7 +4858,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>48</v>
       </c>
@@ -4893,7 +4890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="129" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>48</v>
       </c>
@@ -4925,7 +4922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="130" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>49</v>
       </c>
@@ -4957,7 +4954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>49</v>
       </c>
@@ -4989,7 +4986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>49</v>
       </c>
@@ -5021,7 +5018,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>50</v>
       </c>
@@ -5053,7 +5050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>50</v>
       </c>
@@ -5085,7 +5082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="135" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>50</v>
       </c>
@@ -5117,7 +5114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>50</v>
       </c>
@@ -5149,7 +5146,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>51</v>
       </c>
@@ -5181,7 +5178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="138" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>51</v>
       </c>
@@ -5213,7 +5210,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>51</v>
       </c>
@@ -5245,7 +5242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>51</v>
       </c>
@@ -5277,7 +5274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>52</v>
       </c>
@@ -5309,7 +5306,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>52</v>
       </c>
@@ -5341,7 +5338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="143" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>52</v>
       </c>
@@ -5373,7 +5370,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="144" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>52</v>
       </c>
@@ -5405,7 +5402,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="145" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>52</v>
       </c>
@@ -5437,7 +5434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>52</v>
       </c>
@@ -5469,7 +5466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="147" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>52</v>
       </c>
@@ -5501,7 +5498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="148" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>54</v>
       </c>
@@ -5533,7 +5530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>54</v>
       </c>
@@ -5565,7 +5562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>54</v>
       </c>
@@ -5597,7 +5594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>54</v>
       </c>
@@ -5629,7 +5626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>54</v>
       </c>
@@ -5661,7 +5658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="153" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>54</v>
       </c>
@@ -5693,7 +5690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>54</v>
       </c>
@@ -5725,7 +5722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>56</v>
       </c>
@@ -5757,7 +5754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>56</v>
       </c>
@@ -5789,7 +5786,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="157" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>56</v>
       </c>
@@ -5821,7 +5818,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="158" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>57</v>
       </c>
@@ -5853,7 +5850,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="159" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>57</v>
       </c>
@@ -5885,7 +5882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="160" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>57</v>
       </c>
@@ -5917,7 +5914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="161" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>57</v>
       </c>
@@ -5949,7 +5946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>58</v>
       </c>
@@ -5981,7 +5978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="163" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>58</v>
       </c>
@@ -6013,7 +6010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>58</v>
       </c>
@@ -6045,7 +6042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="165" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>58</v>
       </c>
@@ -6077,7 +6074,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="166" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>58</v>
       </c>
@@ -6109,7 +6106,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="167" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>58</v>
       </c>
@@ -6141,7 +6138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>59</v>
       </c>
@@ -6173,7 +6170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="169" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>59</v>
       </c>
@@ -6205,7 +6202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>59</v>
       </c>
@@ -6237,7 +6234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>59</v>
       </c>
@@ -6269,7 +6266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="172" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>59</v>
       </c>
@@ -6301,7 +6298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>59</v>
       </c>
@@ -6333,7 +6330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>59</v>
       </c>
@@ -6365,7 +6362,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>60</v>
       </c>
@@ -6397,7 +6394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="176" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>60</v>
       </c>
@@ -6429,7 +6426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>60</v>
       </c>
@@ -6461,7 +6458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>60</v>
       </c>
@@ -6493,7 +6490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>60</v>
       </c>
@@ -6525,7 +6522,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>60</v>
       </c>
@@ -6557,7 +6554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>60</v>
       </c>
@@ -6589,7 +6586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>60</v>
       </c>
@@ -6621,7 +6618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>62</v>
       </c>
@@ -6653,7 +6650,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>62</v>
       </c>
@@ -6685,7 +6682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>62</v>
       </c>
@@ -6717,7 +6714,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>63</v>
       </c>
@@ -6749,7 +6746,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>63</v>
       </c>
@@ -6781,7 +6778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>63</v>
       </c>
@@ -6813,7 +6810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>63</v>
       </c>
@@ -6845,7 +6842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>63</v>
       </c>
@@ -6877,7 +6874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>64</v>
       </c>
@@ -6909,7 +6906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>64</v>
       </c>
@@ -6941,7 +6938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>64</v>
       </c>
@@ -6973,7 +6970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="194" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>64</v>
       </c>
@@ -7005,7 +7002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>64</v>
       </c>
@@ -7037,7 +7034,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>64</v>
       </c>
@@ -7069,7 +7066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="197" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>64</v>
       </c>
@@ -7101,7 +7098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>65</v>
       </c>
@@ -7133,7 +7130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="199" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>65</v>
       </c>
@@ -7165,7 +7162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>65</v>
       </c>
@@ -7197,7 +7194,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="201" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>65</v>
       </c>
@@ -7229,7 +7226,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>65</v>
       </c>
@@ -7261,7 +7258,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="203" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>65</v>
       </c>
@@ -7293,7 +7290,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>65</v>
       </c>
@@ -7325,7 +7322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>65</v>
       </c>
@@ -7357,7 +7354,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="206" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>67</v>
       </c>
@@ -7389,7 +7386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>67</v>
       </c>
@@ -7421,7 +7418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="208" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>67</v>
       </c>
@@ -7453,7 +7450,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="209" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>67</v>
       </c>
@@ -7485,7 +7482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="210" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>67</v>
       </c>
@@ -7517,7 +7514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="211" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>67</v>
       </c>
@@ -7549,7 +7546,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="212" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>68</v>
       </c>
@@ -7581,7 +7578,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="213" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>68</v>
       </c>
@@ -7613,7 +7610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="214" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>68</v>
       </c>
@@ -7645,7 +7642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="215" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>68</v>
       </c>
@@ -7677,7 +7674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="216" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>68</v>
       </c>
@@ -7709,7 +7706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="217" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>69</v>
       </c>
@@ -7741,7 +7738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="218" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>69</v>
       </c>
@@ -7773,7 +7770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="219" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>69</v>
       </c>
@@ -7805,7 +7802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="220" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>69</v>
       </c>
@@ -7837,7 +7834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="221" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>69</v>
       </c>
@@ -7869,7 +7866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="222" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>71</v>
       </c>
@@ -7901,7 +7898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="223" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>71</v>
       </c>
@@ -7933,7 +7930,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="224" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>71</v>
       </c>
@@ -7965,7 +7962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="225" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>71</v>
       </c>
@@ -7997,7 +7994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="226" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>71</v>
       </c>
@@ -8029,7 +8026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="227" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>71</v>
       </c>
@@ -8061,7 +8058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="228" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>72</v>
       </c>
@@ -8093,7 +8090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="229" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>72</v>
       </c>
@@ -8125,7 +8122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="230" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>72</v>
       </c>
@@ -8157,7 +8154,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="231" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>72</v>
       </c>
@@ -8189,7 +8186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="232" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>73</v>
       </c>
@@ -8221,7 +8218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="233" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>73</v>
       </c>
@@ -8253,7 +8250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="234" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>73</v>
       </c>
@@ -8285,7 +8282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="235" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>73</v>
       </c>
@@ -8317,7 +8314,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="236" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>73</v>
       </c>
@@ -8349,7 +8346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="237" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>74</v>
       </c>
@@ -8381,7 +8378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="238" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>74</v>
       </c>
@@ -8413,7 +8410,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="239" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>74</v>
       </c>
@@ -8445,7 +8442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="240" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>74</v>
       </c>
@@ -8477,7 +8474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="241" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>74</v>
       </c>
@@ -8509,7 +8506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="242" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>74</v>
       </c>
@@ -8541,7 +8538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="243" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>74</v>
       </c>
@@ -8573,7 +8570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="244" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>75</v>
       </c>
@@ -8605,7 +8602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="245" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>75</v>
       </c>
@@ -8637,7 +8634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="246" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>75</v>
       </c>
@@ -8669,7 +8666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="247" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>75</v>
       </c>
@@ -8701,7 +8698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="248" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>75</v>
       </c>
@@ -8733,7 +8730,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="249" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>76</v>
       </c>
@@ -8765,7 +8762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="250" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>76</v>
       </c>
@@ -8797,7 +8794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="251" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>76</v>
       </c>
@@ -8829,7 +8826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="252" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>76</v>
       </c>
@@ -8861,7 +8858,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="253" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>76</v>
       </c>
@@ -8893,7 +8890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="254" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>77</v>
       </c>
@@ -8925,7 +8922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="255" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>77</v>
       </c>
@@ -8957,7 +8954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="256" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>77</v>
       </c>
@@ -8989,7 +8986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="257" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>78</v>
       </c>
@@ -9021,7 +9018,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="258" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>78</v>
       </c>
@@ -9053,7 +9050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="259" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>78</v>
       </c>
@@ -9085,7 +9082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="260" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>78</v>
       </c>
@@ -9117,7 +9114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="261" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>79</v>
       </c>
@@ -9149,7 +9146,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="262" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>79</v>
       </c>
@@ -9181,7 +9178,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="263" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>79</v>
       </c>
@@ -9213,7 +9210,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="264" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>79</v>
       </c>
@@ -9245,7 +9242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="265" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>81</v>
       </c>
@@ -9277,7 +9274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="266" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>81</v>
       </c>
@@ -9309,7 +9306,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="267" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>81</v>
       </c>
@@ -9341,7 +9338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="268" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>81</v>
       </c>
@@ -9373,7 +9370,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="269" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>81</v>
       </c>
@@ -9405,7 +9402,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="270" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>81</v>
       </c>
@@ -9437,7 +9434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="271" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>81</v>
       </c>
@@ -9469,7 +9466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="272" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>82</v>
       </c>
@@ -9501,7 +9498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="273" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>82</v>
       </c>
@@ -9533,7 +9530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="274" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>82</v>
       </c>
@@ -9565,7 +9562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="275" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>82</v>
       </c>
@@ -9597,7 +9594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="276" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>82</v>
       </c>
@@ -9629,7 +9626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="277" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>82</v>
       </c>
@@ -9661,7 +9658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="278" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>82</v>
       </c>
@@ -9693,7 +9690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="279" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>83</v>
       </c>
@@ -9725,7 +9722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="280" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>83</v>
       </c>
@@ -9757,7 +9754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="281" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>83</v>
       </c>
@@ -9789,7 +9786,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="282" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>83</v>
       </c>
@@ -9821,7 +9818,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="283" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>83</v>
       </c>
@@ -9853,7 +9850,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="284" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>84</v>
       </c>
@@ -9885,7 +9882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="285" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>84</v>
       </c>
@@ -9917,7 +9914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="286" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>84</v>
       </c>
@@ -9949,7 +9946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="287" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>84</v>
       </c>
@@ -9981,7 +9978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="288" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>84</v>
       </c>
@@ -10013,7 +10010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="289" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>85</v>
       </c>
@@ -10045,7 +10042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="290" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>85</v>
       </c>
@@ -10077,7 +10074,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="291" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>85</v>
       </c>
@@ -10109,7 +10106,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="292" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>85</v>
       </c>
@@ -10141,7 +10138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="293" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>85</v>
       </c>
@@ -10173,7 +10170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="294" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>85</v>
       </c>
@@ -10205,7 +10202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="295" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>88</v>
       </c>
@@ -10237,7 +10234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="296" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>88</v>
       </c>
@@ -10269,7 +10266,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="297" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>88</v>
       </c>
@@ -10301,7 +10298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="298" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>90</v>
       </c>
@@ -10333,7 +10330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="299" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>90</v>
       </c>
@@ -10365,7 +10362,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="300" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>90</v>
       </c>
@@ -10397,7 +10394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="301" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>90</v>
       </c>
@@ -10429,7 +10426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="302" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>90</v>
       </c>
@@ -10461,7 +10458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="303" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>90</v>
       </c>
@@ -10493,7 +10490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="304" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>90</v>
       </c>
@@ -10525,7 +10522,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="305" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>90</v>
       </c>
@@ -10557,7 +10554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="306" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>90</v>
       </c>
@@ -10589,7 +10586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="307" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>90</v>
       </c>
@@ -10621,7 +10618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="308" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>91</v>
       </c>
@@ -10653,7 +10650,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="309" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>91</v>
       </c>
@@ -10685,7 +10682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="310" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>91</v>
       </c>
@@ -10717,7 +10714,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="311" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>91</v>
       </c>
@@ -10749,7 +10746,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="312" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>91</v>
       </c>
@@ -10781,7 +10778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="313" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>91</v>
       </c>
@@ -10813,7 +10810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="314" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>91</v>
       </c>
@@ -10845,7 +10842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="315" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>91</v>
       </c>
@@ -10877,7 +10874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="316" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>91</v>
       </c>
@@ -10909,7 +10906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="317" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>92</v>
       </c>
@@ -10941,7 +10938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="318" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>92</v>
       </c>
@@ -10973,7 +10970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="319" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>92</v>
       </c>
@@ -11005,7 +11002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="320" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>92</v>
       </c>
@@ -11037,7 +11034,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="321" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>93</v>
       </c>
@@ -11069,7 +11066,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="322" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>93</v>
       </c>
@@ -11101,7 +11098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="323" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>93</v>
       </c>
@@ -11133,7 +11130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="324" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>93</v>
       </c>
@@ -11165,7 +11162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="325" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>93</v>
       </c>
@@ -11197,7 +11194,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="326" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>94</v>
       </c>
@@ -11229,7 +11226,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="327" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>94</v>
       </c>
@@ -11261,7 +11258,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="328" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>94</v>
       </c>
@@ -11293,7 +11290,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="329" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>94</v>
       </c>
@@ -11325,7 +11322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="330" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>94</v>
       </c>
@@ -11357,7 +11354,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="331" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>95</v>
       </c>
@@ -11389,7 +11386,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="332" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>95</v>
       </c>
@@ -11421,7 +11418,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="333" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>95</v>
       </c>
@@ -11453,7 +11450,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="334" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>95</v>
       </c>
@@ -11485,7 +11482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="335" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>97</v>
       </c>
@@ -11517,7 +11514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="336" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>97</v>
       </c>
@@ -11549,7 +11546,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="337" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>97</v>
       </c>
@@ -11581,7 +11578,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="338" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>97</v>
       </c>
@@ -11613,7 +11610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="339" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>97</v>
       </c>
@@ -11645,7 +11642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="340" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>98</v>
       </c>
@@ -11677,7 +11674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="341" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>98</v>
       </c>
@@ -11709,7 +11706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="342" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>98</v>
       </c>
@@ -11741,7 +11738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="343" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>98</v>
       </c>
@@ -11773,7 +11770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="344" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>99</v>
       </c>
@@ -11805,7 +11802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="345" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>99</v>
       </c>
@@ -11837,7 +11834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="346" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>99</v>
       </c>
@@ -11869,7 +11866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="347" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>99</v>
       </c>
@@ -11901,7 +11898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="348" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>99</v>
       </c>
@@ -11933,7 +11930,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="349" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>99</v>
       </c>
@@ -11965,7 +11962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="350" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>100</v>
       </c>
@@ -11997,7 +11994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="351" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>100</v>
       </c>
@@ -12029,7 +12026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="352" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>100</v>
       </c>
@@ -12061,7 +12058,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="353" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>100</v>
       </c>
@@ -12093,7 +12090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="354" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>100</v>
       </c>
@@ -12125,7 +12122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="355" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>100</v>
       </c>
@@ -12157,7 +12154,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="356" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>100</v>
       </c>
@@ -12189,7 +12186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="357" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>100</v>
       </c>
@@ -12221,7 +12218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="358" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>100</v>
       </c>
@@ -12253,7 +12250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="359" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>101</v>
       </c>
@@ -12285,7 +12282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="360" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>101</v>
       </c>
@@ -12317,7 +12314,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="361" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>101</v>
       </c>
@@ -12349,7 +12346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="362" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>102</v>
       </c>
@@ -12381,7 +12378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="363" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>102</v>
       </c>
@@ -12413,7 +12410,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="364" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>102</v>
       </c>
@@ -12445,7 +12442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="365" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>103</v>
       </c>
@@ -12477,7 +12474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="366" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>103</v>
       </c>
@@ -12509,7 +12506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="367" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>103</v>
       </c>
@@ -12541,7 +12538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="368" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>104</v>
       </c>
@@ -12573,7 +12570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="369" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>104</v>
       </c>
@@ -12605,7 +12602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="370" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>104</v>
       </c>
@@ -12637,7 +12634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="371" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>104</v>
       </c>
@@ -12669,7 +12666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="372" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>104</v>
       </c>
@@ -12701,7 +12698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="373" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>104</v>
       </c>
@@ -12733,7 +12730,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="374" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>104</v>
       </c>
@@ -12765,7 +12762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="375" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>105</v>
       </c>
@@ -12797,7 +12794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="376" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>105</v>
       </c>
@@ -12829,7 +12826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="377" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>105</v>
       </c>
@@ -12861,7 +12858,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="378" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>105</v>
       </c>
@@ -12893,7 +12890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="379" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>105</v>
       </c>
@@ -12925,7 +12922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="380" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>106</v>
       </c>
@@ -12957,7 +12954,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="381" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>106</v>
       </c>
@@ -12989,7 +12986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="382" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>106</v>
       </c>
@@ -13021,7 +13018,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="383" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>106</v>
       </c>
@@ -13053,7 +13050,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="384" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>106</v>
       </c>
@@ -13085,7 +13082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="385" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>106</v>
       </c>
@@ -13117,7 +13114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="386" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>106</v>
       </c>
@@ -13149,7 +13146,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="387" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>106</v>
       </c>
@@ -13181,7 +13178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="388" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>108</v>
       </c>
@@ -13213,7 +13210,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="389" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>108</v>
       </c>
@@ -13245,7 +13242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="390" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>108</v>
       </c>
@@ -13277,7 +13274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="391" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>108</v>
       </c>
@@ -13309,7 +13306,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="392" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>108</v>
       </c>
@@ -13341,7 +13338,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="393" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>108</v>
       </c>
@@ -13373,7 +13370,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="394" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>108</v>
       </c>
@@ -13405,7 +13402,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="395" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>108</v>
       </c>
@@ -13437,7 +13434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="396" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>108</v>
       </c>
@@ -13469,7 +13466,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="397" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>111</v>
       </c>
@@ -13501,7 +13498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="398" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>111</v>
       </c>
@@ -13533,7 +13530,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="399" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>111</v>
       </c>
@@ -13565,7 +13562,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="400" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>111</v>
       </c>
@@ -13597,7 +13594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="401" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>111</v>
       </c>
@@ -13629,7 +13626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="402" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>111</v>
       </c>
@@ -13661,7 +13658,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="403" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>111</v>
       </c>
@@ -13693,7 +13690,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="404" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>113</v>
       </c>
@@ -13725,7 +13722,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="405" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>113</v>
       </c>
@@ -13757,7 +13754,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="406" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>113</v>
       </c>
@@ -13789,7 +13786,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="407" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>113</v>
       </c>
@@ -13821,7 +13818,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="408" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>113</v>
       </c>
@@ -13853,7 +13850,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="409" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>114</v>
       </c>
@@ -13885,7 +13882,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="410" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>114</v>
       </c>
@@ -13917,7 +13914,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="411" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>114</v>
       </c>
@@ -13949,7 +13946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="412" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>114</v>
       </c>
@@ -13981,7 +13978,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="413" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>115</v>
       </c>
@@ -14013,7 +14010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="414" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>115</v>
       </c>
@@ -14045,7 +14042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="415" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>115</v>
       </c>
@@ -14077,7 +14074,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="416" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>116</v>
       </c>
@@ -14109,7 +14106,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="417" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>116</v>
       </c>
@@ -14141,7 +14138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="418" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>116</v>
       </c>
@@ -14173,7 +14170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="419" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>116</v>
       </c>
@@ -14205,7 +14202,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="420" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>116</v>
       </c>
@@ -14237,7 +14234,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="421" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>117</v>
       </c>
@@ -14269,7 +14266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="422" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>117</v>
       </c>
@@ -14301,7 +14298,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="423" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>117</v>
       </c>
@@ -14333,7 +14330,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="424" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>117</v>
       </c>
@@ -14365,7 +14362,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="425" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>117</v>
       </c>
@@ -14397,7 +14394,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="426" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>117</v>
       </c>
@@ -14429,7 +14426,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="427" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>117</v>
       </c>
@@ -14461,7 +14458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="428" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>118</v>
       </c>
@@ -14493,7 +14490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="429" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>118</v>
       </c>
@@ -14525,7 +14522,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="430" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>118</v>
       </c>
@@ -14557,7 +14554,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="431" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>118</v>
       </c>
@@ -14589,7 +14586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="432" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>119</v>
       </c>
@@ -14621,7 +14618,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="433" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>119</v>
       </c>
@@ -14653,7 +14650,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="434" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>119</v>
       </c>
@@ -14685,7 +14682,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="435" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>119</v>
       </c>
@@ -14717,7 +14714,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="436" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>119</v>
       </c>
@@ -14749,7 +14746,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="437" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>119</v>
       </c>
@@ -14781,7 +14778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="438" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>119</v>
       </c>
@@ -14813,7 +14810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="439" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>120</v>
       </c>
@@ -14845,7 +14842,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="440" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>120</v>
       </c>
@@ -14877,7 +14874,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="441" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>120</v>
       </c>
@@ -14909,7 +14906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="442" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>120</v>
       </c>
@@ -14941,7 +14938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="443" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>120</v>
       </c>
@@ -14973,7 +14970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="444" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>121</v>
       </c>
@@ -15005,7 +15002,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="445" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>121</v>
       </c>
@@ -15037,7 +15034,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="446" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>121</v>
       </c>
@@ -15069,7 +15066,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="447" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>121</v>
       </c>
@@ -15101,7 +15098,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="448" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>121</v>
       </c>
@@ -15133,7 +15130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="449" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>123</v>
       </c>
@@ -15165,7 +15162,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="450" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>123</v>
       </c>
@@ -15197,7 +15194,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="451" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>123</v>
       </c>
@@ -15229,7 +15226,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="452" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>123</v>
       </c>
@@ -15261,7 +15258,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="453" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>123</v>
       </c>
@@ -15293,7 +15290,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="454" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>123</v>
       </c>
@@ -15325,7 +15322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="455" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>123</v>
       </c>
@@ -15357,7 +15354,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="456" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>126</v>
       </c>
@@ -15389,7 +15386,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="457" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>126</v>
       </c>
@@ -15421,7 +15418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="458" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>126</v>
       </c>
@@ -15453,7 +15450,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="459" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>126</v>
       </c>
@@ -15485,7 +15482,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="460" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>126</v>
       </c>
@@ -15517,7 +15514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="461" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>126</v>
       </c>
@@ -15549,7 +15546,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="462" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>128</v>
       </c>
@@ -15581,7 +15578,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="463" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>128</v>
       </c>
@@ -15613,7 +15610,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="464" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>128</v>
       </c>
@@ -15645,7 +15642,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="465" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>128</v>
       </c>
@@ -15677,7 +15674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="466" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>128</v>
       </c>
@@ -15709,7 +15706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="467" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>128</v>
       </c>
@@ -15741,7 +15738,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="468" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>128</v>
       </c>
@@ -15773,7 +15770,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="469" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>130</v>
       </c>
@@ -15805,7 +15802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="470" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>130</v>
       </c>
@@ -15837,7 +15834,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="471" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>130</v>
       </c>
@@ -15869,7 +15866,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="472" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>130</v>
       </c>
@@ -15901,7 +15898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="473" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>130</v>
       </c>
@@ -15933,7 +15930,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="474" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>130</v>
       </c>
@@ -15965,7 +15962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="475" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>130</v>
       </c>
@@ -15997,7 +15994,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="476" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>132</v>
       </c>
@@ -16029,7 +16026,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="477" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>132</v>
       </c>
@@ -16061,7 +16058,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="478" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>132</v>
       </c>
@@ -16093,7 +16090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="479" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>132</v>
       </c>
@@ -16125,7 +16122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="480" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>132</v>
       </c>
@@ -16157,7 +16154,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="481" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>132</v>
       </c>
@@ -16189,7 +16186,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="482" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>132</v>
       </c>
@@ -16221,7 +16218,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="483" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>134</v>
       </c>
@@ -16253,7 +16250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="484" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>134</v>
       </c>
@@ -16285,7 +16282,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="485" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>134</v>
       </c>
@@ -16317,7 +16314,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="486" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>134</v>
       </c>
@@ -16349,7 +16346,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="487" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>134</v>
       </c>
@@ -16381,7 +16378,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="488" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>134</v>
       </c>
@@ -16413,7 +16410,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="489" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>135</v>
       </c>
@@ -16445,7 +16442,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="490" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>135</v>
       </c>
@@ -16477,7 +16474,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="491" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>135</v>
       </c>
@@ -16509,7 +16506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="492" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>135</v>
       </c>
@@ -16541,7 +16538,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="493" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>135</v>
       </c>
@@ -16573,7 +16570,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="494" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>136</v>
       </c>
@@ -16605,7 +16602,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="495" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>136</v>
       </c>
@@ -16637,7 +16634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="496" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>136</v>
       </c>
@@ -16669,7 +16666,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="497" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>136</v>
       </c>
@@ -16701,7 +16698,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="498" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>136</v>
       </c>
@@ -16733,7 +16730,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="499" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>136</v>
       </c>
@@ -16765,7 +16762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="500" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>139</v>
       </c>
@@ -16797,7 +16794,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="501" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>139</v>
       </c>
@@ -16829,7 +16826,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="502" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>139</v>
       </c>
@@ -16861,7 +16858,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="503" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="503" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>139</v>
       </c>
@@ -16893,7 +16890,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="504" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>140</v>
       </c>
@@ -16925,7 +16922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="505" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="505" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>140</v>
       </c>
@@ -16957,7 +16954,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="506" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="506" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>140</v>
       </c>
@@ -16989,7 +16986,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="507" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="507" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>140</v>
       </c>
@@ -17021,7 +17018,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="508" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>140</v>
       </c>
@@ -17053,7 +17050,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="509" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="509" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>140</v>
       </c>
@@ -17085,7 +17082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="510" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>142</v>
       </c>
@@ -17117,7 +17114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="511" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="511" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>142</v>
       </c>
@@ -17149,7 +17146,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="512" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="512" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>142</v>
       </c>
@@ -17181,7 +17178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="513" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>142</v>
       </c>
@@ -17213,7 +17210,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="514" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="514" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>142</v>
       </c>
@@ -17245,7 +17242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="515" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="515" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>142</v>
       </c>
@@ -17277,7 +17274,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="516" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="516" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>142</v>
       </c>
@@ -17309,7 +17306,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="517" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="517" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>142</v>
       </c>
@@ -17341,7 +17338,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="518" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="518" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>142</v>
       </c>
@@ -17373,7 +17370,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="519" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="519" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>144</v>
       </c>
@@ -17405,7 +17402,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="520" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="520" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>144</v>
       </c>
@@ -17437,7 +17434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="521" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="521" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>145</v>
       </c>
@@ -17469,7 +17466,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="522" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="522" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>145</v>
       </c>
@@ -17501,7 +17498,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="523" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="523" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>145</v>
       </c>
@@ -17533,7 +17530,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="524" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="524" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>145</v>
       </c>
@@ -17579,9 +17576,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>147</v>
       </c>
@@ -17593,7 +17590,7 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>